<commit_message>
limpieza de archivos previo a acabar el semestre
</commit_message>
<xml_diff>
--- a/Inteligencia de negocios/trabajo 16 12 probabilidad BI condicional.xlsx
+++ b/Inteligencia de negocios/trabajo 16 12 probabilidad BI condicional.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMPANY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMPANY\Documents\Archivos_Sexto_semestre\Inteligencia de negocios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E609EFFD-F544-474D-98FD-09C47DBB04C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A909F-CADF-4D2B-AC6A-3599AF032C44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="195" windowWidth="12780" windowHeight="10020" activeTab="2" xr2:uid="{E715C966-273A-493D-962B-54EA66958103}"/>
+    <workbookView xWindow="7905" yWindow="285" windowWidth="12780" windowHeight="10020" activeTab="1" xr2:uid="{E715C966-273A-493D-962B-54EA66958103}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>day = weekday</t>
   </si>
@@ -186,13 +186,22 @@
   </si>
   <si>
     <t>4.6 las 4 preguntas ejercicios</t>
+  </si>
+  <si>
+    <t>Cap3.1.1</t>
+  </si>
+  <si>
+    <t>Cap3.1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +211,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -263,10 +279,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -285,9 +302,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3242,14 +3261,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF82922-8D99-4CC4-A6A4-F8C3A4F910EC}">
   <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="10" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3502,6 +3522,25 @@
         <f>+DATA!F12/DATA!$F$3</f>
         <v>0</v>
       </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="10">
+        <f>+B4*B9*B13*B17*B18</f>
+        <v>3.9358600583090375E-3</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" ref="H11:J11" si="0">+C4*C9*C13*C17*C18</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -3522,6 +3561,9 @@
       <c r="E12" s="6">
         <f>+DATA!F13/DATA!$F$3</f>
         <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3691,7 +3733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DF36B6-FA57-4AF1-B7AE-C36301B08FF9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>